<commit_message>
commit in test branch
</commit_message>
<xml_diff>
--- a/02 Doc/Link Doc.xlsx
+++ b/02 Doc/Link Doc.xlsx
@@ -387,13 +387,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="2" max="2" width="43.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">

</xml_diff>

<commit_message>
update link doc in show branch
</commit_message>
<xml_diff>
--- a/02 Doc/Link Doc.xlsx
+++ b/02 Doc/Link Doc.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Scrum" sheetId="1" r:id="rId1"/>
     <sheet name="MRN" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Wave3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -424,6 +424,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,18 +446,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modify link doc in show branch
</commit_message>
<xml_diff>
--- a/02 Doc/Link Doc.xlsx
+++ b/02 Doc/Link Doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>http://it-ea-agile-test:7070/browse/CBSSCRM</t>
   </si>
@@ -25,6 +25,9 @@
   </si>
   <si>
     <t>http://it-ea-agile-test:7070/secure/RapidBoard.jspa?rapidView=1648&amp;useStoredSettings=true</t>
+  </si>
+  <si>
+    <t>Baidu</t>
   </si>
 </sst>
 </file>
@@ -438,10 +441,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>